<commit_message>
DR's quant data updated
</commit_message>
<xml_diff>
--- a/data/countries/dominican_republic/Dominican Republic_quantitative_3Jun25.xlsx
+++ b/data/countries/dominican_republic/Dominican Republic_quantitative_3Jun25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:D196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,10 +441,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Document</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>dates</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>quants</t>
         </is>
@@ -456,8 +461,13 @@
           <t>Objetivo especifíco 1.1.2</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -465,8 +475,13 @@
           <t>Línea de acción 1.1.2.3</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -474,8 +489,13 @@
           <t>Objetivo especifíco 1.3.1</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -483,8 +503,13 @@
           <t>Línea de acción 1.3.1.4</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -492,8 +517,13 @@
           <t>Objetivo específico 2.3.3</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -501,8 +531,13 @@
           <t>Línea de acción 2.3.3.4</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -510,8 +545,13 @@
           <t>Objetivo específico 2.4.1</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -519,8 +559,13 @@
           <t>Línea de acción 2.4.1.2</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -528,8 +573,13 @@
           <t>Línea de acción 2.4.1.3</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -537,8 +587,13 @@
           <t>Línea de acción 2.4.1.4</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -546,8 +601,13 @@
           <t>Línea de acción 2.4.1.5</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -555,8 +615,13 @@
           <t>Línea de acción 2.4.1.7</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -564,8 +629,13 @@
           <t>Objetivo específico 2.4.2</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -573,8 +643,13 @@
           <t>Línea de acción 2.4.2.3</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -582,8 +657,13 @@
           <t>Línea de acción 2.4.2.6</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -591,8 +671,13 @@
           <t>Objetivo específico 2.4.3</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -600,8 +685,13 @@
           <t>Línea de acción 2.4.3.6</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -609,8 +699,13 @@
           <t>Objetivo específico 3.2.1</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -618,8 +713,13 @@
           <t>Línea de acción 3.2.1.1</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -627,8 +727,13 @@
           <t>Línea de acción 3.2.1.2</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -636,8 +741,13 @@
           <t>Línea de acción 3.2.1.4</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -645,8 +755,13 @@
           <t>Línea de acción 3.2.1.5</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -654,8 +769,13 @@
           <t>Línea de acción 3.2.1.6</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -663,8 +783,13 @@
           <t>Objetivo específico 3.2.2</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -672,8 +797,13 @@
           <t>Línea de acción 3.2.2.1</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -681,8 +811,13 @@
           <t>Línea de acción 3.2.2.2</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -690,8 +825,13 @@
           <t>Línea de acción 3.2.2.4</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -699,8 +839,13 @@
           <t>Línea de acción 3.2.2.5</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -708,8 +853,13 @@
           <t>Línea de acción 3.2.2.6</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -717,8 +867,13 @@
           <t>Línea de acción 3.5.3.2</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -726,8 +881,13 @@
           <t>Línea de acción 3.5.3.3</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -735,8 +895,13 @@
           <t>Línea de acción 3.5.3.4</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -744,8 +909,13 @@
           <t>Objetivo específico 3.5.4</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -753,8 +923,13 @@
           <t>Objetivo específico 3.5.5</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -762,8 +937,13 @@
           <t>Línea de acción 3.5.5.1</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -771,8 +951,13 @@
           <t>Línea de acción 3.5.5.2</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -780,8 +965,13 @@
           <t>Línea de acción 3.5.5.3</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -789,8 +979,13 @@
           <t>Línea de acción 3.5.5.4</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -798,8 +993,13 @@
           <t>Objetivo especifíco 4.1.1</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -807,8 +1007,13 @@
           <t>Objetivo especifíco 4.1.2</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -816,8 +1021,13 @@
           <t>Objetivo especifíco 4.1.3</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -825,8 +1035,13 @@
           <t>Objetivo especifíco 4.1.4</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -834,8 +1049,13 @@
           <t>Objetivo especifíco 4.2.1</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -843,8 +1063,13 @@
           <t>Objetivo especifíco 4.3.1</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Ley 1- 12 Estrategia Nacional de Desarrollo</t>
+        </is>
+      </c>
       <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -854,10 +1079,15 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2020</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>para el 2010</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -865,8 +1095,13 @@
           <t>Objetivo estratégico B</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2021</t>
+        </is>
+      </c>
       <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -874,8 +1109,13 @@
           <t>Objetivo estratégico C</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2022</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -883,8 +1123,13 @@
           <t>Objetivo estratégico D</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2023</t>
+        </is>
+      </c>
       <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -894,10 +1139,15 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2024</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -907,10 +1157,15 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2025</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -920,10 +1175,15 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2026</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>Para el 2020</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -933,10 +1193,15 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2027</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -946,10 +1211,15 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2028</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>25%</t>
         </is>
@@ -963,10 +1233,15 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2029</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -976,10 +1251,15 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2030</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -989,10 +1269,15 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2031</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1002,10 +1287,15 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2032</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1015,10 +1305,15 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2033</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1028,10 +1323,15 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2034</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1041,10 +1341,15 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2035</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1054,10 +1359,15 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2036</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1067,10 +1377,15 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2037</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1080,10 +1395,15 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2038</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1093,10 +1413,15 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2039</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
           <t>Para el 2015</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1106,10 +1431,15 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2040</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1119,10 +1449,15 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2041</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1132,10 +1467,15 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2042</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1145,10 +1485,15 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>Estrategia nacional de conservación y uso Sostenible de la Biodiversidad 2011-2043</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
           <t>Para el 2016</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1156,8 +1501,13 @@
           <t>Objetivo de Mitigación 1.1</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1165,8 +1515,13 @@
           <t>Objetivo de Mitigación 1.2</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr"/>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1174,8 +1529,13 @@
           <t>Objetivo de Mitigación 1.3</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr"/>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1183,8 +1543,13 @@
           <t>Objetivo de Mitigación 1.4</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1192,8 +1557,13 @@
           <t>Objetivo de Mitigación 1.5</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr"/>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1201,8 +1571,13 @@
           <t>Objetivo de Mitigación 1.6</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr"/>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1210,8 +1585,13 @@
           <t>Objetivo de Mitigación 1.7</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1219,8 +1599,13 @@
           <t>Objetivo de Mitigación 1.8</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr"/>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1228,8 +1613,13 @@
           <t>Objetivo de Mitigación 1.9</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1237,8 +1627,13 @@
           <t>Objetivo de Mitigación 1.10</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1246,8 +1641,13 @@
           <t>Objetivo de Mitigación 1.11</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1255,8 +1655,13 @@
           <t>Objetivo de Mitigación 1.12</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr"/>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1264,8 +1669,13 @@
           <t>Objetivo de Mitigación 1.13</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr"/>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1273,8 +1683,13 @@
           <t>Objetivo de Mitigación 1.14</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr"/>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1282,8 +1697,13 @@
           <t>Objetivo de Mitigación 1.15</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr"/>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1291,8 +1711,13 @@
           <t>Objetivo de Mitigación 1.16</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr"/>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1300,8 +1725,13 @@
           <t>Objetivo de Mitigación 1.17</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr"/>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1309,8 +1739,13 @@
           <t>Objetivo de Mitigación 1.18</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr"/>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1318,8 +1753,13 @@
           <t>Objetivo de Mitigación 1.19</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr"/>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1327,8 +1767,13 @@
           <t>Objetivo de Mitigación 1.20</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr">
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
         <is>
           <t>100%</t>
         </is>
@@ -1340,8 +1785,13 @@
           <t>Objetivo de Mitigación 1.21</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr"/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1349,8 +1799,13 @@
           <t>Objetivo de Mitigación 1.22</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr"/>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1358,8 +1813,13 @@
           <t>Objetivo de Mitigación 1.23</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr"/>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1367,8 +1827,13 @@
           <t>Objetivo de Mitigación 1.24</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr">
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
         <is>
           <t>100%</t>
         </is>
@@ -1380,8 +1845,13 @@
           <t>Objetivo de Mitigación 1.25</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1389,8 +1859,13 @@
           <t>Objetivo de Mitigación 1.26</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1398,8 +1873,13 @@
           <t>Objetivo de Mitigación 1.27</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1407,8 +1887,13 @@
           <t>Objetivo de Mitigación 1.28</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1416,8 +1901,13 @@
           <t>Objetivo de Mitigación 1.29</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr"/>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1425,8 +1915,13 @@
           <t>Objetivo de Mitigación 1.30</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr"/>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1434,8 +1929,13 @@
           <t>Objetivo de Mitigación 1.31</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr"/>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1443,8 +1943,13 @@
           <t>Objetivo de Mitigación 1.32</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr"/>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1452,8 +1957,13 @@
           <t>Objetivo de Mitigación 1.33</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1463,10 +1973,15 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
           <t>para 2035</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
+      <c r="D103" t="inlineStr">
         <is>
           <t>75,102 ha; 5 MM</t>
         </is>
@@ -1480,10 +1995,15 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
           <t>10 años</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
+      <c r="D104" t="inlineStr">
         <is>
           <t>146,648 Ha; 2.2 MM</t>
         </is>
@@ -1497,10 +2017,15 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
           <t>hasta 2023</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr">
+      <c r="D105" t="inlineStr">
         <is>
           <t>15,000 ha; 43,750 ha</t>
         </is>
@@ -1512,8 +2037,13 @@
           <t>Objetivo de Mitigación 1.37</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1521,8 +2051,13 @@
           <t>Objetivo de Mitigación 1.38</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -1530,8 +2065,13 @@
           <t>Objetivo de Mitigación 1.39</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr"/>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -1539,8 +2079,13 @@
           <t>Objetivo de Mitigación 1.40</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -1550,10 +2095,15 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
           <t>30 años</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr">
+      <c r="D110" t="inlineStr">
         <is>
           <t>30,000 ha</t>
         </is>
@@ -1565,8 +2115,13 @@
           <t>Objetivo de Mitigación 1.42</t>
         </is>
       </c>
-      <c r="B111" t="inlineStr"/>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -1574,8 +2129,13 @@
           <t>Objetivo de Mitigación 1.43</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr"/>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -1583,8 +2143,13 @@
           <t>Objetivo de Mitigación 1.44</t>
         </is>
       </c>
-      <c r="B113" t="inlineStr"/>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -1592,8 +2157,13 @@
           <t>Objetivo de Mitigación 1.45</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr"/>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -1601,8 +2171,13 @@
           <t>Objetivo de Mitigación 1.46</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr"/>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -1610,8 +2185,13 @@
           <t>Medidas de adaptación 2.1</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr"/>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -1619,8 +2199,13 @@
           <t>Medidas de adaptación 2.2</t>
         </is>
       </c>
-      <c r="B117" t="inlineStr"/>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -1628,8 +2213,13 @@
           <t>Medidas de adaptación 2.3</t>
         </is>
       </c>
-      <c r="B118" t="inlineStr"/>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -1637,8 +2227,13 @@
           <t>Medidas de adaptación 2.4</t>
         </is>
       </c>
-      <c r="B119" t="inlineStr"/>
-      <c r="C119" t="inlineStr">
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr">
         <is>
           <t>dos</t>
         </is>
@@ -1650,8 +2245,13 @@
           <t>Medidas de adaptación 2.5</t>
         </is>
       </c>
-      <c r="B120" t="inlineStr"/>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -1659,8 +2259,13 @@
           <t>Medidas de adaptación 2.6</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr"/>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -1668,8 +2273,13 @@
           <t>Medidas de adaptación 2.7</t>
         </is>
       </c>
-      <c r="B122" t="inlineStr"/>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -1677,8 +2287,13 @@
           <t>Medidas de adaptación 2.8</t>
         </is>
       </c>
-      <c r="B123" t="inlineStr"/>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -1686,8 +2301,13 @@
           <t>Medidas de adaptación 2.9</t>
         </is>
       </c>
-      <c r="B124" t="inlineStr"/>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -1695,8 +2315,13 @@
           <t>Medidas de adaptación 2.10</t>
         </is>
       </c>
-      <c r="B125" t="inlineStr"/>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -1704,8 +2329,13 @@
           <t>Medidas de adaptación 2.11</t>
         </is>
       </c>
-      <c r="B126" t="inlineStr"/>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -1713,8 +2343,13 @@
           <t>Medidas de adaptación 2.12</t>
         </is>
       </c>
-      <c r="B127" t="inlineStr"/>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -1722,8 +2357,13 @@
           <t>Medidas de adaptación 2.13</t>
         </is>
       </c>
-      <c r="B128" t="inlineStr"/>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -1731,8 +2371,13 @@
           <t>Medidas de adaptación 2.14</t>
         </is>
       </c>
-      <c r="B129" t="inlineStr"/>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -1740,8 +2385,13 @@
           <t>Medidas de adaptación 2.15</t>
         </is>
       </c>
-      <c r="B130" t="inlineStr"/>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -1749,8 +2399,13 @@
           <t>Medidas de adaptación 2.16</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr"/>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -1758,8 +2413,13 @@
           <t>Medidas de adaptación 2.17</t>
         </is>
       </c>
-      <c r="B132" t="inlineStr"/>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -1767,8 +2427,13 @@
           <t>Medidas de adaptación 2.18</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr"/>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -1776,8 +2441,13 @@
           <t>Medidas de adaptación 2.19</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr"/>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -1785,8 +2455,13 @@
           <t>Medidas de adaptación 2.20</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr"/>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -1794,8 +2469,13 @@
           <t>Medidas de adaptación 2.21</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr"/>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -1803,8 +2483,13 @@
           <t>Medidas de adaptación 2.22</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr"/>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -1812,8 +2497,13 @@
           <t>Medidas de adaptación 2.23</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr"/>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -1821,8 +2511,13 @@
           <t>Medidas de adaptación 2.24</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr"/>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C139" t="inlineStr"/>
+      <c r="D139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -1830,8 +2525,13 @@
           <t>Medidas de adaptación 2.25</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr"/>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C140" t="inlineStr"/>
+      <c r="D140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -1839,8 +2539,13 @@
           <t>Medidas de adaptación 2.26</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr"/>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -1848,8 +2553,13 @@
           <t>Medidas de adaptación 2.27</t>
         </is>
       </c>
-      <c r="B142" t="inlineStr"/>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -1857,8 +2567,13 @@
           <t>Medidas de adaptación 2.28</t>
         </is>
       </c>
-      <c r="B143" t="inlineStr"/>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -1866,8 +2581,13 @@
           <t>Medidas de adaptación 2.29</t>
         </is>
       </c>
-      <c r="B144" t="inlineStr"/>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -1875,8 +2595,13 @@
           <t>Medidas de adaptación 2.30</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr"/>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -1884,8 +2609,13 @@
           <t>Medidas de adaptación 2.31</t>
         </is>
       </c>
-      <c r="B146" t="inlineStr"/>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -1893,8 +2623,13 @@
           <t>Medidas de adaptación 2.32</t>
         </is>
       </c>
-      <c r="B147" t="inlineStr"/>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -1902,8 +2637,13 @@
           <t>Medidas de adaptación 2.33</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr"/>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -1911,8 +2651,13 @@
           <t>Medidas de adaptación 2.34</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr"/>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -1920,8 +2665,13 @@
           <t>Medidas de adaptación 2.35</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr"/>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -1929,8 +2679,13 @@
           <t>Medidas de adaptación 2.36</t>
         </is>
       </c>
-      <c r="B151" t="inlineStr"/>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -1938,8 +2693,13 @@
           <t>Medidas de adaptación 2.37</t>
         </is>
       </c>
-      <c r="B152" t="inlineStr"/>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -1949,10 +2709,15 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
           <t>Al 2030</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -1962,10 +2727,15 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
           <t>Al 2030</t>
         </is>
       </c>
-      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -1975,10 +2745,15 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
           <t>Al 2030</t>
         </is>
       </c>
-      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -1988,10 +2763,15 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
           <t>Al 2030</t>
         </is>
       </c>
-      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2001,10 +2781,15 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
           <t>Para 2024</t>
         </is>
       </c>
-      <c r="C157" t="inlineStr">
+      <c r="D157" t="inlineStr">
         <is>
           <t>200</t>
         </is>
@@ -2016,8 +2801,13 @@
           <t>Acción para el Empoderamiento Climatico 4.6</t>
         </is>
       </c>
-      <c r="B158" t="inlineStr"/>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -2025,8 +2815,13 @@
           <t>Acción para el Empoderamiento Climatico 4.7</t>
         </is>
       </c>
-      <c r="B159" t="inlineStr"/>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C159" t="inlineStr"/>
+      <c r="D159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -2034,8 +2829,13 @@
           <t>Acción para el Empoderamiento Climatico 4.8</t>
         </is>
       </c>
-      <c r="B160" t="inlineStr"/>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -2043,8 +2843,13 @@
           <t>Acción para el Empoderamiento Climatico 4.9</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr"/>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -2052,8 +2857,13 @@
           <t>Acción para el Empoderamiento Climatico 4.10</t>
         </is>
       </c>
-      <c r="B162" t="inlineStr"/>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -2061,8 +2871,13 @@
           <t>Acción para el Empoderamiento Climatico 4.11</t>
         </is>
       </c>
-      <c r="B163" t="inlineStr"/>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -2072,10 +2887,15 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
           <t>Al 2022</t>
         </is>
       </c>
-      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -2085,10 +2905,15 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
           <t>Al 2030</t>
         </is>
       </c>
-      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -2098,10 +2923,15 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
           <t>Al 2022</t>
         </is>
       </c>
-      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -2109,8 +2939,13 @@
           <t>Acción para el Empoderamiento Climatico 4.15</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr"/>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -2118,8 +2953,13 @@
           <t>Acción para el Empoderamiento Climatico 4.16</t>
         </is>
       </c>
-      <c r="B168" t="inlineStr"/>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -2127,8 +2967,13 @@
           <t>Acción para el Empoderamiento Climatico 4.17</t>
         </is>
       </c>
-      <c r="B169" t="inlineStr"/>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -2136,8 +2981,13 @@
           <t>Acción para el Empoderamiento Climatico 4.18</t>
         </is>
       </c>
-      <c r="B170" t="inlineStr"/>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -2145,8 +2995,13 @@
           <t>Acción para el Empoderamiento Climatico 4.19</t>
         </is>
       </c>
-      <c r="B171" t="inlineStr"/>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -2154,8 +3009,13 @@
           <t>Acción para el Empoderamiento Climatico 4.20</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr"/>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -2163,8 +3023,13 @@
           <t>Acción para el Empoderamiento Climatico 4.21</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr"/>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -2172,8 +3037,13 @@
           <t>Acción para el Empoderamiento Climatico 4.22</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr"/>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C174" t="inlineStr"/>
+      <c r="D174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -2183,10 +3053,15 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
           <t>Al 2021</t>
         </is>
       </c>
-      <c r="C175" t="inlineStr"/>
+      <c r="D175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -2194,8 +3069,13 @@
           <t>Elementos Transversales 5.1</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr"/>
-      <c r="C176" t="inlineStr">
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr">
         <is>
           <t>nueve</t>
         </is>
@@ -2207,8 +3087,13 @@
           <t>Elementos Transversales 5.2</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr"/>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -2216,8 +3101,13 @@
           <t>Elementos Transversales 5.3</t>
         </is>
       </c>
-      <c r="B178" t="inlineStr"/>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C178" t="inlineStr"/>
+      <c r="D178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -2225,8 +3115,13 @@
           <t>Elementos Transversales 5.4</t>
         </is>
       </c>
-      <c r="B179" t="inlineStr"/>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C179" t="inlineStr"/>
+      <c r="D179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -2234,8 +3129,13 @@
           <t>Elementos Transversales 5.5</t>
         </is>
       </c>
-      <c r="B180" t="inlineStr"/>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C180" t="inlineStr"/>
+      <c r="D180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -2243,8 +3143,13 @@
           <t>Elementos Transversales 5.6</t>
         </is>
       </c>
-      <c r="B181" t="inlineStr"/>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C181" t="inlineStr"/>
+      <c r="D181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -2252,8 +3157,13 @@
           <t>Elementos Transversales 5.7</t>
         </is>
       </c>
-      <c r="B182" t="inlineStr"/>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C182" t="inlineStr"/>
+      <c r="D182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -2261,8 +3171,13 @@
           <t>Elementos Transversales 5.8</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr"/>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C183" t="inlineStr"/>
+      <c r="D183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -2270,8 +3185,13 @@
           <t>Elementos Transversales 5.9</t>
         </is>
       </c>
-      <c r="B184" t="inlineStr"/>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C184" t="inlineStr"/>
+      <c r="D184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -2279,8 +3199,13 @@
           <t>Elementos Transversales 5.10</t>
         </is>
       </c>
-      <c r="B185" t="inlineStr"/>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C185" t="inlineStr"/>
+      <c r="D185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -2288,8 +3213,13 @@
           <t>Elementos Transversales 5.11</t>
         </is>
       </c>
-      <c r="B186" t="inlineStr"/>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C186" t="inlineStr"/>
+      <c r="D186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -2297,8 +3227,13 @@
           <t>Elementos Transversales 5.12</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr"/>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C187" t="inlineStr"/>
+      <c r="D187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -2306,8 +3241,13 @@
           <t>Elementos Transversales 5.13</t>
         </is>
       </c>
-      <c r="B188" t="inlineStr"/>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C188" t="inlineStr"/>
+      <c r="D188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -2315,8 +3255,13 @@
           <t>Elementos Transversales 5.14</t>
         </is>
       </c>
-      <c r="B189" t="inlineStr"/>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C189" t="inlineStr"/>
+      <c r="D189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -2324,8 +3269,13 @@
           <t>Elementos Transversales 5.15</t>
         </is>
       </c>
-      <c r="B190" t="inlineStr"/>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C190" t="inlineStr"/>
+      <c r="D190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -2333,8 +3283,13 @@
           <t>Gobernanza Climática 6.1</t>
         </is>
       </c>
-      <c r="B191" t="inlineStr"/>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C191" t="inlineStr"/>
+      <c r="D191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -2342,8 +3297,13 @@
           <t>Gobernanza Climática 6.2</t>
         </is>
       </c>
-      <c r="B192" t="inlineStr"/>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C192" t="inlineStr"/>
+      <c r="D192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -2351,8 +3311,13 @@
           <t>Gobernanza Climática 6.3</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr"/>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C193" t="inlineStr"/>
+      <c r="D193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -2360,8 +3325,13 @@
           <t>Gobernanza Climática 6.4</t>
         </is>
       </c>
-      <c r="B194" t="inlineStr"/>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C194" t="inlineStr"/>
+      <c r="D194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -2369,8 +3339,13 @@
           <t>Gobernanza Climática 6.5</t>
         </is>
       </c>
-      <c r="B195" t="inlineStr"/>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C195" t="inlineStr"/>
+      <c r="D195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -2378,8 +3353,13 @@
           <t>Gobernanza Climática 6.6</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr"/>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>NDC-RD 2020</t>
+        </is>
+      </c>
       <c r="C196" t="inlineStr"/>
+      <c r="D196" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>